<commit_message>
json and format templates
</commit_message>
<xml_diff>
--- a/CourseProposal/json_output/instructional_methods_description_dataframe.xlsx
+++ b/CourseProposal/json_output/instructional_methods_description_dataframe.xlsx
@@ -1,75 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Instructional Method</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Classroom</t>
-  </si>
-  <si>
-    <t>Peer Sharing</t>
-  </si>
-  <si>
-    <t>Group Discussion</t>
-  </si>
-  <si>
-    <t>Case Study</t>
-  </si>
-  <si>
-    <t>Classroom instruction, involving lectures and presentations, is essential for establishing a strong foundation. It allows for the efficient and structured delivery of core concepts, ensuring all learners receive a consistent understanding of the methods and procedures central to security risk analysis.</t>
-  </si>
-  <si>
-    <t>Peer sharing provides an opportunity for learners to learn from each other's experiences and insights. By discussing real-world scenarios and challenges, learners can broaden their perspectives and gain a deeper appreciation for the complexities involved in identifying and addressing security risks.</t>
-  </si>
-  <si>
-    <t>Group discussions encourage active participation and collaborative problem-solving. By working together to analyze potential security threats and develop mitigation strategies, learners can enhance their critical thinking skills and learn to leverage the diverse expertise within a security team.</t>
-  </si>
-  <si>
-    <t>Case studies offer realistic scenarios that learners can analyze to apply their knowledge and skills. By examining specific instances of security breaches or vulnerabilities, learners can develop their ability to identify risks, assess potential impacts, and recommend appropriate corrective actions, thereby bridging the gap between theory and practice.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,54 +420,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Instructional Method</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Interactive Presentation</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Interactive Presentation is an ideal instructional method for this course as it allows learners to engage actively with the content related to generative AI and storytelling. By incorporating interactive elements, such as real-time AI tool demonstrations and audience participation, learners can better understand complex concepts like AI-generated script ideation and ethical considerations. This method fosters an engaging learning environment where learners can ask questions and receive immediate feedback, enhancing their grasp of narrative structures and AI applications in media.</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Brainstorming</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Brainstorming is particularly suitable for this course as it encourages creative thinking and collaboration among learners. When developing compelling script elements or identifying effective prompt terms for AI-generated storyboards, brainstorming sessions allow learners to explore diverse ideas and perspectives. This method supports the iterative process of refining AI-generated content by enabling learners to collectively generate innovative solutions and enhance their understanding of narrative components and visual storytelling techniques.</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Demonstration</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Demonstration is a crucial instructional method for this course, as it provides learners with a visual and hands-on approach to understanding generative AI tools and techniques. By demonstrating how to use AI tools for script development, storyboarding, and video creation, learners can see the practical application of theoretical concepts. This method helps learners grasp complex processes, such as refining video scripts for clarity and tone, by breaking them down into manageable steps and showcasing real-time results, thereby enhancing their learning experience.</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Drill and Practice</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Drill and Practice is an effective instructional method for reinforcing learners' understanding of AI-generated content and ethical considerations. By providing opportunities for learners to practice applying AI tools and techniques in a controlled environment, they can refine their skills and knowledge. This method helps learners build confidence in their ability to analyze AI outputs for bias and copyright risks, apply corrective actions, and develop best practices for ethical AI content generation. Through repeated practice, learners can better prepare for real-world challenges in media production.</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>